<commit_message>
Remove old BANKNIFTY expiry logic; use Fyers option chain only
</commit_message>
<xml_diff>
--- a/logs/trade_status_history.xlsx
+++ b/logs/trade_status_history.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,6 +664,80 @@
         <v>-645.7499999999995</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-23 22:44:23</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NSE:BANKNIFTY25OCT58400CE</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>258.15</v>
+      </c>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="n">
+        <v>243.15</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>243.15</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>288.15</v>
+      </c>
+      <c r="H6" s="3" t="inlineStr"/>
+      <c r="I6" s="3" t="n">
+        <v>339.5000000000016</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>3.75750532636066</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>61.25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-31 10:31:45</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NSE:BANKNIFTY25NOV57900PE</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>539.5</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>569.55</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>524.5</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>554.55</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>569.5</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>1051.749999999998</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>1051.749999999998</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>5.569972196478212</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>-257.2500000000008</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>